<commit_message>
[FBL-21] - Import excel data & create player, staff templates
</commit_message>
<xml_diff>
--- a/public/templates/add_players_template.xlsx
+++ b/public/templates/add_players_template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35DCCF24-84A0-4488-9A2B-CB5407D5ECF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B028324F-11AC-4A3E-88C3-A5EA0D477D83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{85EA4461-1249-4D6A-B536-FBBD987C4F6A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{D152182D-1F00-43E0-B8E8-C4F06ED7C6F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,24 +36,66 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
-  <si>
-    <t>STT</t>
-  </si>
-  <si>
-    <t>Họ Tên</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+  <si>
+    <t>Đây là trang hướng dẫn</t>
+  </si>
+  <si>
+    <t>Sheet2 là trang chứa dữ liệu, khi submit, không được đổi tên Sheet2</t>
+  </si>
+  <si>
+    <t>Ý nghĩa các trường thông tin như sau</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Số thứ tự</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Tên cầu thủ</t>
+  </si>
+  <si>
+    <t>IdNumber</t>
+  </si>
+  <si>
+    <t>Số định danh (ví dụ như số CMND)</t>
+  </si>
+  <si>
+    <t>Nationality</t>
+  </si>
+  <si>
+    <t>Quốc tịch của cầu thủ</t>
+  </si>
+  <si>
+    <t>StripNumber</t>
   </si>
   <si>
     <t>Số áo thi đấu</t>
   </si>
   <si>
+    <t>Position</t>
+  </si>
+  <si>
     <t>Vị trí thi đấu</t>
   </si>
   <si>
-    <t>Số định danh</t>
-  </si>
-  <si>
-    <t>Quốc tịch</t>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Huy</t>
+  </si>
+  <si>
+    <t>Anh</t>
+  </si>
+  <si>
+    <t>GK</t>
+  </si>
+  <si>
+    <t>Loại cầu thủ, nếu là ngoại binh thì nhập 1, ngược lại nhập 0</t>
   </si>
 </sst>
 </file>
@@ -84,7 +127,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -92,13 +135,33 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -412,42 +475,178 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2DC07B4-05B4-479A-A419-104D331B1FBD}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{03A6D6EB-0091-46A7-AAAB-47D1CAA27C9B}">
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="4" width="18.28515625" customWidth="1"/>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="54.28515625" customWidth="1"/>
+    <col min="3" max="4" width="18.28515625" customWidth="1"/>
     <col min="5" max="5" width="18.85546875" customWidth="1"/>
     <col min="6" max="6" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="1" t="s">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>3</v>
+      <c r="B6" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E686111-7A96-4972-A0E2-715C884CA810}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
+    <col min="3" max="3" width="18.140625" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="6" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2">
+        <v>12312312323</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" s="6">
+        <v>1</v>
+      </c>
+      <c r="F2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="textLength" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1" xr:uid="{2701D3D4-06D5-4EA4-A953-AB42176379B9}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hướng dẫn" prompt="Số áo lớn hơn 0" sqref="E1:E1048576" xr:uid="{76D69604-01F4-4276-8EA0-36EF49084407}">
+      <formula1>0</formula1>
+    </dataValidation>
+    <dataValidation type="textLength" operator="greaterThanOrEqual" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hướng dẫn" prompt="Tối thiểu 9 kí tự" sqref="C1:C1048576" xr:uid="{000DB3E5-B6F0-4D9D-864B-9C74B993D406}">
+      <formula1>9</formula1>
+    </dataValidation>
+    <dataValidation type="decimal" allowBlank="1" showInputMessage="1" showErrorMessage="1" promptTitle="Hướng dẫn" prompt="1 là ngoại binh, 0 là trong nước" sqref="G1:G1048576" xr:uid="{E955FA9A-833E-4C11-9B57-DD202DC15FF9}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>